<commit_message>
KSOE-Layout code, compared btw original and with virtual stock in yard 1
</commit_message>
<xml_diff>
--- a/data/process_gis_mapping_table.xlsx
+++ b/data/process_gis_mapping_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sohyon\PycharmProjects\KSOE-Layout\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C848EDA-52D2-4108-A524-AE3D511C9846}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDEDF156-E63A-4B91-B9BB-EA93636E4883}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{17952004-864D-4D8F-9198-5430A7F4D83F}"/>
+    <workbookView xWindow="624" yWindow="384" windowWidth="10956" windowHeight="16272" xr2:uid="{17952004-864D-4D8F-9198-5430A7F4D83F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="92">
   <si>
     <t>선각공장</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -135,17 +135,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1도크쉘터</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2도크쉘터</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3도크쉘터</t>
-  </si>
-  <si>
     <t>의장쉘터</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -382,6 +371,26 @@
   </si>
   <si>
     <t>LOC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1도크PE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2도크PE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3도크PE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8도크PE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9도크PE</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -746,10 +755,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAC94349-53C5-419B-9059-C59911026147}">
-  <dimension ref="A1:C61"/>
+  <dimension ref="A1:C63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -759,13 +768,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
@@ -773,10 +782,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
@@ -784,10 +793,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
@@ -795,10 +804,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
@@ -806,10 +815,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.4">
@@ -817,10 +826,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.4">
@@ -839,10 +848,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C8" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.4">
@@ -905,10 +914,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C14" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.4">
@@ -916,10 +925,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C15" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.4">
@@ -927,10 +936,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C16" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.4">
@@ -938,10 +947,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C17" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.4">
@@ -949,10 +958,10 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C18" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.4">
@@ -960,10 +969,10 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C19" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.4">
@@ -971,10 +980,10 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C20" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.4">
@@ -982,10 +991,10 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C21" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.4">
@@ -993,10 +1002,10 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C22" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.4">
@@ -1004,10 +1013,10 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C23" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.4">
@@ -1015,10 +1024,10 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C24" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.4">
@@ -1026,10 +1035,10 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C25" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.4">
@@ -1037,10 +1046,10 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C26" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.4">
@@ -1048,10 +1057,10 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C27" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.4">
@@ -1059,373 +1068,395 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C28" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
-        <v>27</v>
+        <v>87</v>
       </c>
       <c r="B29" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="C29" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>88</v>
       </c>
       <c r="B30" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="C30" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
-        <v>29</v>
+        <v>89</v>
       </c>
       <c r="B31" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="C31" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B32" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C32" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B33" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C33" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B34" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C34" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B35" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C35" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B36" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C36" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B37" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C37" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B38" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C38" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B39" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C39" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B40" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C40" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B41" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C41" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B42" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C42" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B43" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C43" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A44" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B44" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C44" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A45" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B45" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C45" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B46" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C46" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A47" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B47" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C47" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A48" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B48" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C48" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A49" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B49" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C49" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A50" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B50" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C50" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A51" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B51" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C51" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A52" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B52" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C52" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A53" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B53" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C53" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A54" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B54" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C54" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A55" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B55" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C55" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A56" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B56" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C56" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A57" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B57" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C57" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A58" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B58" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C58" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A59" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B59" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C59" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A60" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B60" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C60" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A61" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B61" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C61" t="s">
-        <v>59</v>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A62" t="s">
+        <v>90</v>
+      </c>
+      <c r="B62" t="s">
+        <v>10</v>
+      </c>
+      <c r="C62" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A63" t="s">
+        <v>91</v>
+      </c>
+      <c r="B63" t="s">
+        <v>11</v>
+      </c>
+      <c r="C63" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>